<commit_message>
Resolve multiple surnames issue
</commit_message>
<xml_diff>
--- a/nhl-fantasy-rankings-2023.xlsx
+++ b/nhl-fantasy-rankings-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\nhl-fantasy-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E6DA8E-94E9-48A3-8476-CC6051A7F7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42923F2D-DF9C-4255-83A6-32FF941B0144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5955" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5955" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NHL.com" sheetId="1" r:id="rId1"/>
@@ -386,6 +386,9 @@
     <t>Jeremy Swayman</t>
   </si>
   <si>
+    <t>Joel Eriksson Ek</t>
+  </si>
+  <si>
     <t>Vince Dunn</t>
   </si>
   <si>
@@ -918,9 +921,6 @@
   </si>
   <si>
     <t>Jacob Trouba</t>
-  </si>
-  <si>
-    <t>Joel Eriksson Ek</t>
   </si>
   <si>
     <t>MON</t>
@@ -1528,13 +1528,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="25.3125" customWidth="1"/>
+    <col min="2" max="2" width="21.3671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2704,7 +2704,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>299</v>
+        <v>121</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
@@ -2718,13 +2718,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C85" t="s">
         <v>38</v>
       </c>
       <c r="D85" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2732,7 +2732,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C86" t="s">
         <v>92</v>
@@ -2746,7 +2746,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C87" t="s">
         <v>22</v>
@@ -2760,7 +2760,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C88" t="s">
         <v>41</v>
@@ -2774,7 +2774,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C89" t="s">
         <v>38</v>
@@ -2788,7 +2788,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C90" t="s">
         <v>38</v>
@@ -2802,7 +2802,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C91" t="s">
         <v>19</v>
@@ -2816,7 +2816,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C92" t="s">
         <v>41</v>
@@ -2830,7 +2830,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C93" t="s">
         <v>57</v>
@@ -2844,7 +2844,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
@@ -2858,7 +2858,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C95" t="s">
         <v>57</v>
@@ -2872,7 +2872,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -2886,7 +2886,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C97" t="s">
         <v>41</v>
@@ -2900,7 +2900,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C98" t="s">
         <v>41</v>
@@ -2914,7 +2914,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C99" t="s">
         <v>12</v>
@@ -2928,7 +2928,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C100" t="s">
         <v>22</v>
@@ -2942,7 +2942,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C101" t="s">
         <v>57</v>
@@ -2956,7 +2956,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C102" t="s">
         <v>41</v>
@@ -2970,7 +2970,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C103" t="s">
         <v>57</v>
@@ -2984,7 +2984,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C104" t="s">
         <v>5</v>
@@ -2998,7 +2998,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C105" t="s">
         <v>38</v>
@@ -3012,7 +3012,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C106" t="s">
         <v>41</v>
@@ -3026,7 +3026,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C107" t="s">
         <v>41</v>
@@ -3040,7 +3040,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C108" t="s">
         <v>57</v>
@@ -3054,7 +3054,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C109" t="s">
         <v>38</v>
@@ -3068,7 +3068,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C110" t="s">
         <v>19</v>
@@ -3082,7 +3082,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C111" t="s">
         <v>22</v>
@@ -3096,7 +3096,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C112" t="s">
         <v>41</v>
@@ -3110,7 +3110,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C113" t="s">
         <v>5</v>
@@ -3124,7 +3124,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C114" t="s">
         <v>38</v>
@@ -3138,7 +3138,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C115" t="s">
         <v>5</v>
@@ -3152,7 +3152,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C116" t="s">
         <v>38</v>
@@ -3166,7 +3166,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C117" t="s">
         <v>38</v>
@@ -3180,13 +3180,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C118" t="s">
         <v>22</v>
       </c>
       <c r="D118" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3194,7 +3194,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C119" t="s">
         <v>41</v>
@@ -3208,7 +3208,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C120" t="s">
         <v>38</v>
@@ -3222,13 +3222,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C121" t="s">
         <v>5</v>
       </c>
       <c r="D121" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3236,13 +3236,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C122" t="s">
         <v>19</v>
       </c>
       <c r="D122" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3250,7 +3250,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C123" t="s">
         <v>38</v>
@@ -3264,7 +3264,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C124" t="s">
         <v>19</v>
@@ -3278,13 +3278,13 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C125" t="s">
         <v>57</v>
       </c>
       <c r="D125" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3292,7 +3292,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C126" t="s">
         <v>22</v>
@@ -3306,7 +3306,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -3320,13 +3320,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C128" t="s">
         <v>8</v>
       </c>
       <c r="D128" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3334,7 +3334,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C129" t="s">
         <v>5</v>
@@ -3348,7 +3348,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C130" t="s">
         <v>92</v>
@@ -3362,7 +3362,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -3376,7 +3376,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C132" t="s">
         <v>5</v>
@@ -3390,7 +3390,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C133" t="s">
         <v>22</v>
@@ -3404,7 +3404,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C134" t="s">
         <v>22</v>
@@ -3418,7 +3418,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C135" t="s">
         <v>12</v>
@@ -3432,13 +3432,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C136" t="s">
         <v>57</v>
       </c>
       <c r="D136" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3446,7 +3446,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C137" t="s">
         <v>38</v>
@@ -3460,7 +3460,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C138" t="s">
         <v>57</v>
@@ -3474,7 +3474,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C139" t="s">
         <v>38</v>
@@ -3488,7 +3488,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C140" t="s">
         <v>57</v>
@@ -3502,13 +3502,13 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C141" t="s">
         <v>5</v>
       </c>
       <c r="D141" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3516,13 +3516,13 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C142" t="s">
         <v>5</v>
       </c>
       <c r="D142" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3530,7 +3530,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C143" t="s">
         <v>5</v>
@@ -3544,7 +3544,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C144" t="s">
         <v>41</v>
@@ -3558,7 +3558,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C145" t="s">
         <v>41</v>
@@ -3572,7 +3572,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C146" t="s">
         <v>38</v>
@@ -3586,7 +3586,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C147" t="s">
         <v>38</v>
@@ -3600,7 +3600,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C148" t="s">
         <v>92</v>
@@ -3614,7 +3614,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C149" t="s">
         <v>38</v>
@@ -3628,7 +3628,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C150" t="s">
         <v>5</v>
@@ -3642,7 +3642,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C151" t="s">
         <v>57</v>
@@ -3656,7 +3656,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C152" t="s">
         <v>5</v>
@@ -3670,7 +3670,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C153" t="s">
         <v>22</v>
@@ -3684,7 +3684,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C154" t="s">
         <v>19</v>
@@ -3698,7 +3698,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C155" t="s">
         <v>22</v>
@@ -3712,13 +3712,13 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C156" t="s">
         <v>57</v>
       </c>
       <c r="D156" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3726,7 +3726,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C157" t="s">
         <v>41</v>
@@ -3740,7 +3740,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C158" t="s">
         <v>38</v>
@@ -3754,7 +3754,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C159" t="s">
         <v>41</v>
@@ -3768,7 +3768,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C160" t="s">
         <v>38</v>
@@ -3782,13 +3782,13 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C161" t="s">
         <v>38</v>
       </c>
       <c r="D161" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3796,13 +3796,13 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C162" t="s">
         <v>8</v>
       </c>
       <c r="D162" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3810,7 +3810,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C163" t="s">
         <v>38</v>
@@ -3824,7 +3824,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C164" t="s">
         <v>38</v>
@@ -3838,7 +3838,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C165" t="s">
         <v>19</v>
@@ -3852,7 +3852,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C166" t="s">
         <v>5</v>
@@ -3866,7 +3866,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C167" t="s">
         <v>41</v>
@@ -3880,7 +3880,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C168" t="s">
         <v>12</v>
@@ -3894,7 +3894,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C169" t="s">
         <v>8</v>
@@ -3908,7 +3908,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C170" t="s">
         <v>12</v>
@@ -3922,13 +3922,13 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C171" t="s">
         <v>5</v>
       </c>
       <c r="D171" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3936,7 +3936,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C172" t="s">
         <v>12</v>
@@ -3950,7 +3950,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C173" t="s">
         <v>41</v>
@@ -3964,7 +3964,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C174" t="s">
         <v>57</v>
@@ -3978,7 +3978,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C175" t="s">
         <v>8</v>
@@ -3992,7 +3992,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C176" t="s">
         <v>57</v>
@@ -4006,7 +4006,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C177" t="s">
         <v>5</v>
@@ -4020,7 +4020,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C178" t="s">
         <v>57</v>
@@ -4034,7 +4034,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C179" t="s">
         <v>19</v>
@@ -4048,7 +4048,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C180" t="s">
         <v>5</v>
@@ -4062,7 +4062,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C181" t="s">
         <v>38</v>
@@ -4076,7 +4076,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C182" t="s">
         <v>38</v>
@@ -4090,7 +4090,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C183" t="s">
         <v>41</v>
@@ -4104,7 +4104,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C184" t="s">
         <v>41</v>
@@ -4118,13 +4118,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C185" t="s">
         <v>12</v>
       </c>
       <c r="D185" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4132,7 +4132,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C186" t="s">
         <v>41</v>
@@ -4146,7 +4146,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C187" t="s">
         <v>57</v>
@@ -4160,7 +4160,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C188" t="s">
         <v>12</v>
@@ -4174,7 +4174,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C189" t="s">
         <v>38</v>
@@ -4188,13 +4188,13 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C190" t="s">
         <v>8</v>
       </c>
       <c r="D190" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4202,7 +4202,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C191" t="s">
         <v>12</v>
@@ -4216,7 +4216,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C192" t="s">
         <v>38</v>
@@ -4230,7 +4230,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C193" t="s">
         <v>38</v>
@@ -4244,7 +4244,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C194" t="s">
         <v>5</v>
@@ -4258,7 +4258,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C195" t="s">
         <v>22</v>
@@ -4272,13 +4272,13 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C196" t="s">
         <v>5</v>
       </c>
       <c r="D196" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4286,13 +4286,13 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
+        <v>240</v>
+      </c>
+      <c r="C197" t="s">
+        <v>5</v>
+      </c>
+      <c r="D197" t="s">
         <v>239</v>
-      </c>
-      <c r="C197" t="s">
-        <v>5</v>
-      </c>
-      <c r="D197" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4300,7 +4300,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C198" t="s">
         <v>41</v>
@@ -4314,7 +4314,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C199" t="s">
         <v>57</v>
@@ -4328,13 +4328,13 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C200" t="s">
         <v>41</v>
       </c>
       <c r="D200" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4342,13 +4342,13 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C201" t="s">
         <v>38</v>
       </c>
       <c r="D201" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4356,7 +4356,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C202" t="s">
         <v>38</v>
@@ -4370,7 +4370,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C203" t="s">
         <v>8</v>
@@ -4384,7 +4384,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C204" t="s">
         <v>5</v>
@@ -4398,7 +4398,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C205" t="s">
         <v>38</v>
@@ -4412,7 +4412,7 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C206" t="s">
         <v>38</v>
@@ -4426,13 +4426,13 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C207" t="s">
         <v>5</v>
       </c>
       <c r="D207" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4440,7 +4440,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C208" t="s">
         <v>19</v>
@@ -4454,13 +4454,13 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C209" t="s">
         <v>8</v>
       </c>
       <c r="D209" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4468,7 +4468,7 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C210" t="s">
         <v>8</v>
@@ -4482,7 +4482,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C211" t="s">
         <v>38</v>
@@ -4496,7 +4496,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C212" t="s">
         <v>22</v>
@@ -4510,7 +4510,7 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C213" t="s">
         <v>38</v>
@@ -4524,13 +4524,13 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C214" t="s">
         <v>38</v>
       </c>
       <c r="D214" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4538,7 +4538,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C215" t="s">
         <v>12</v>
@@ -4552,13 +4552,13 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C216" t="s">
         <v>41</v>
       </c>
       <c r="D216" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4566,7 +4566,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C217" t="s">
         <v>19</v>
@@ -4580,7 +4580,7 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C218" t="s">
         <v>57</v>
@@ -4594,13 +4594,13 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C219" t="s">
         <v>38</v>
       </c>
       <c r="D219" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4608,7 +4608,7 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C220" t="s">
         <v>38</v>
@@ -4622,13 +4622,13 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C221" t="s">
         <v>57</v>
       </c>
       <c r="D221" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4636,7 +4636,7 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C222" t="s">
         <v>12</v>
@@ -4650,13 +4650,13 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C223" t="s">
         <v>57</v>
       </c>
       <c r="D223" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4664,13 +4664,13 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C224" t="s">
         <v>12</v>
       </c>
       <c r="D224" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4678,13 +4678,13 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C225" t="s">
         <v>5</v>
       </c>
       <c r="D225" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4692,7 +4692,7 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C226" t="s">
         <v>57</v>
@@ -4706,7 +4706,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C227" t="s">
         <v>57</v>
@@ -4720,7 +4720,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C228" t="s">
         <v>41</v>
@@ -4734,7 +4734,7 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C229" t="s">
         <v>57</v>
@@ -4748,7 +4748,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C230" t="s">
         <v>8</v>
@@ -4762,7 +4762,7 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C231" t="s">
         <v>92</v>
@@ -4776,7 +4776,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C232" t="s">
         <v>38</v>
@@ -4790,7 +4790,7 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C233" t="s">
         <v>38</v>
@@ -4804,7 +4804,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C234" t="s">
         <v>22</v>
@@ -4818,7 +4818,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C235" t="s">
         <v>57</v>
@@ -4832,7 +4832,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C236" t="s">
         <v>8</v>
@@ -4846,13 +4846,13 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C237" t="s">
         <v>12</v>
       </c>
       <c r="D237" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4860,7 +4860,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C238" t="s">
         <v>5</v>
@@ -4874,7 +4874,7 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C239" t="s">
         <v>12</v>
@@ -4888,7 +4888,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C240" t="s">
         <v>57</v>
@@ -4902,13 +4902,13 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C241" t="s">
         <v>19</v>
       </c>
       <c r="D241" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4916,7 +4916,7 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C242" t="s">
         <v>38</v>
@@ -4930,13 +4930,13 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C243" t="s">
         <v>5</v>
       </c>
       <c r="D243" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -4944,7 +4944,7 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C244" t="s">
         <v>5</v>
@@ -4958,7 +4958,7 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C245" t="s">
         <v>5</v>
@@ -4972,7 +4972,7 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C246" t="s">
         <v>41</v>
@@ -4986,7 +4986,7 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C247" t="s">
         <v>5</v>
@@ -5000,13 +5000,13 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C248" t="s">
         <v>38</v>
       </c>
       <c r="D248" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5014,7 +5014,7 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C249" t="s">
         <v>92</v>
@@ -5028,7 +5028,7 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C250" t="s">
         <v>19</v>
@@ -5042,7 +5042,7 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C251" t="s">
         <v>38</v>
@@ -5060,13 +5060,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="B268" sqref="B268"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="31.89453125" customWidth="1"/>
+    <col min="2" max="2" width="24.1015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5262,7 +5260,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5298,7 +5296,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -5416,7 +5414,7 @@
         <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5444,7 +5442,7 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5500,7 +5498,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5522,13 +5520,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5536,7 +5534,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
@@ -5578,7 +5576,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -5648,7 +5646,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
@@ -5682,7 +5680,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5774,13 +5772,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5788,7 +5786,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
         <v>12</v>
@@ -5808,7 +5806,7 @@
         <v>41</v>
       </c>
       <c r="D53" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5830,13 +5828,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C55" t="s">
         <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5858,7 +5856,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -5872,7 +5870,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C58" t="s">
         <v>38</v>
@@ -5934,7 +5932,7 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5956,13 +5954,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
         <v>12</v>
       </c>
       <c r="D64" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5970,7 +5968,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>299</v>
+        <v>121</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -5984,13 +5982,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6004,7 +6002,7 @@
         <v>38</v>
       </c>
       <c r="D67" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6012,13 +6010,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C68" t="s">
         <v>38</v>
       </c>
       <c r="D68" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6068,13 +6066,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C72" t="s">
         <v>38</v>
       </c>
       <c r="D72" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6088,7 +6086,7 @@
         <v>38</v>
       </c>
       <c r="D73" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6096,7 +6094,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C74" t="s">
         <v>38</v>
@@ -6124,7 +6122,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C76" t="s">
         <v>38</v>
@@ -6138,7 +6136,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C77" t="s">
         <v>12</v>
@@ -6152,7 +6150,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C78" t="s">
         <v>41</v>
@@ -6180,7 +6178,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" t="s">
         <v>41</v>
@@ -6194,7 +6192,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
@@ -6214,7 +6212,7 @@
         <v>19</v>
       </c>
       <c r="D82" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6222,13 +6220,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C83" t="s">
         <v>12</v>
       </c>
       <c r="D83" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6236,7 +6234,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
@@ -6264,13 +6262,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C86" t="s">
         <v>19</v>
       </c>
       <c r="D86" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6278,13 +6276,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C87" t="s">
         <v>12</v>
       </c>
       <c r="D87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6326,7 +6324,7 @@
         <v>12</v>
       </c>
       <c r="D90" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6354,7 +6352,7 @@
         <v>38</v>
       </c>
       <c r="D92" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6362,7 +6360,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C93" t="s">
         <v>38</v>
@@ -6376,7 +6374,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
@@ -6488,13 +6486,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C102" t="s">
         <v>12</v>
       </c>
       <c r="D102" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6502,7 +6500,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C103" t="s">
         <v>38</v>
@@ -6530,7 +6528,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C105" t="s">
         <v>19</v>
@@ -6544,7 +6542,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C106" t="s">
         <v>19</v>
@@ -6558,13 +6556,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C107" t="s">
         <v>38</v>
       </c>
       <c r="D107" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6572,13 +6570,13 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C108" t="s">
         <v>12</v>
       </c>
       <c r="D108" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6600,13 +6598,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C110" t="s">
         <v>38</v>
       </c>
       <c r="D110" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6620,7 +6618,7 @@
         <v>19</v>
       </c>
       <c r="D111" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6628,13 +6626,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C112" t="s">
         <v>41</v>
       </c>
       <c r="D112" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6642,7 +6640,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C113" t="s">
         <v>41</v>
@@ -6656,7 +6654,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C114" t="s">
         <v>5</v>
@@ -6670,7 +6668,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C115" t="s">
         <v>41</v>
@@ -6684,7 +6682,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C116" t="s">
         <v>5</v>
@@ -6698,7 +6696,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C117" t="s">
         <v>38</v>
@@ -6712,7 +6710,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C118" t="s">
         <v>38</v>
@@ -6754,7 +6752,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C121" t="s">
         <v>5</v>
@@ -6768,13 +6766,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C122" t="s">
         <v>5</v>
       </c>
       <c r="D122" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6788,7 +6786,7 @@
         <v>5</v>
       </c>
       <c r="D123" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6838,7 +6836,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C127" t="s">
         <v>19</v>
@@ -6858,7 +6856,7 @@
         <v>5</v>
       </c>
       <c r="D128" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6866,7 +6864,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C129" t="s">
         <v>38</v>
@@ -6880,7 +6878,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C130" t="s">
         <v>38</v>
@@ -6894,7 +6892,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -6908,7 +6906,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C132" t="s">
         <v>38</v>
@@ -6922,7 +6920,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C133" t="s">
         <v>12</v>
@@ -6936,7 +6934,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C134" t="s">
         <v>5</v>
@@ -6950,13 +6948,13 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C135" t="s">
         <v>5</v>
       </c>
       <c r="D135" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6964,7 +6962,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C136" t="s">
         <v>12</v>
@@ -6978,7 +6976,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C137" t="s">
         <v>19</v>
@@ -6992,7 +6990,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C138" t="s">
         <v>19</v>
@@ -7006,7 +7004,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C139" t="s">
         <v>19</v>
@@ -7034,7 +7032,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C141" t="s">
         <v>12</v>
@@ -7048,7 +7046,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C142" t="s">
         <v>38</v>
@@ -7090,7 +7088,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C145" t="s">
         <v>38</v>
@@ -7104,7 +7102,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C146" t="s">
         <v>12</v>
@@ -7118,7 +7116,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C147" t="s">
         <v>38</v>
@@ -7132,7 +7130,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C148" t="s">
         <v>19</v>
@@ -7146,7 +7144,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C149" t="s">
         <v>12</v>
@@ -7160,7 +7158,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C150" t="s">
         <v>19</v>
@@ -7174,7 +7172,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C151" t="s">
         <v>38</v>
@@ -7216,7 +7214,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C154" t="s">
         <v>38</v>
@@ -7230,7 +7228,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C155" t="s">
         <v>5</v>
@@ -7258,13 +7256,13 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C157" t="s">
         <v>41</v>
       </c>
       <c r="D157" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7272,7 +7270,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C158" t="s">
         <v>5</v>
@@ -7286,13 +7284,13 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C159" t="s">
         <v>19</v>
       </c>
       <c r="D159" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7314,7 +7312,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C161" t="s">
         <v>41</v>
@@ -7328,7 +7326,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C162" t="s">
         <v>19</v>
@@ -7356,7 +7354,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C164" t="s">
         <v>38</v>
@@ -7370,7 +7368,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C165" t="s">
         <v>38</v>
@@ -7384,7 +7382,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C166" t="s">
         <v>12</v>
@@ -7412,7 +7410,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C168" t="s">
         <v>5</v>
@@ -7426,7 +7424,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C169" t="s">
         <v>5</v>
@@ -7440,7 +7438,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C170" t="s">
         <v>41</v>
@@ -7454,7 +7452,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C171" t="s">
         <v>19</v>
@@ -7468,7 +7466,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C172" t="s">
         <v>12</v>
@@ -7482,7 +7480,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C173" t="s">
         <v>38</v>
@@ -7496,13 +7494,13 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C174" t="s">
         <v>5</v>
       </c>
       <c r="D174" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7510,13 +7508,13 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C175" t="s">
         <v>5</v>
       </c>
       <c r="D175" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7524,7 +7522,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C176" t="s">
         <v>5</v>
@@ -7538,13 +7536,13 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C177" t="s">
         <v>38</v>
       </c>
       <c r="D177" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7580,7 +7578,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C180" t="s">
         <v>19</v>
@@ -7594,7 +7592,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C181" t="s">
         <v>5</v>
@@ -7664,7 +7662,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C186" t="s">
         <v>5</v>
@@ -7678,7 +7676,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C187" t="s">
         <v>5</v>
@@ -7692,7 +7690,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C188" t="s">
         <v>5</v>
@@ -7712,7 +7710,7 @@
         <v>38</v>
       </c>
       <c r="D189" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7720,7 +7718,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C190" t="s">
         <v>12</v>
@@ -7734,7 +7732,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C191" t="s">
         <v>38</v>
@@ -7748,7 +7746,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C192" t="s">
         <v>5</v>
@@ -7762,7 +7760,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C193" t="s">
         <v>12</v>
@@ -7776,7 +7774,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C194" t="s">
         <v>38</v>
@@ -7804,13 +7802,13 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C196" t="s">
         <v>12</v>
       </c>
       <c r="D196" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7852,7 +7850,7 @@
         <v>38</v>
       </c>
       <c r="D199" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7874,7 +7872,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C201" t="s">
         <v>38</v>
@@ -7888,7 +7886,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C202" t="s">
         <v>38</v>
@@ -7922,7 +7920,7 @@
         <v>38</v>
       </c>
       <c r="D204" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7950,7 +7948,7 @@
         <v>12</v>
       </c>
       <c r="D206" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7958,13 +7956,13 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C207" t="s">
         <v>41</v>
       </c>
       <c r="D207" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -7986,7 +7984,7 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C209" t="s">
         <v>19</v>
@@ -8014,7 +8012,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C211" t="s">
         <v>38</v>
@@ -8056,7 +8054,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C214" t="s">
         <v>41</v>
@@ -8070,7 +8068,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C215" t="s">
         <v>38</v>
@@ -8098,7 +8096,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C217" t="s">
         <v>38</v>
@@ -8182,7 +8180,7 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C223" t="s">
         <v>12</v>
@@ -8272,7 +8270,7 @@
         <v>38</v>
       </c>
       <c r="D229" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8280,7 +8278,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C230" t="s">
         <v>5</v>
@@ -8300,7 +8298,7 @@
         <v>5</v>
       </c>
       <c r="D231" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8308,7 +8306,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C232" t="s">
         <v>5</v>
@@ -8336,13 +8334,13 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C234" t="s">
         <v>5</v>
       </c>
       <c r="D234" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8356,7 +8354,7 @@
         <v>38</v>
       </c>
       <c r="D235" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8364,7 +8362,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C236" t="s">
         <v>5</v>
@@ -8378,7 +8376,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C237" t="s">
         <v>41</v>
@@ -8392,7 +8390,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C238" t="s">
         <v>38</v>
@@ -8406,13 +8404,13 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C239" t="s">
         <v>41</v>
       </c>
       <c r="D239" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8420,7 +8418,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C240" t="s">
         <v>5</v>
@@ -8434,7 +8432,7 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C241" t="s">
         <v>19</v>
@@ -8462,7 +8460,7 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C243" t="s">
         <v>19</v>
@@ -8476,13 +8474,13 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C244" t="s">
         <v>5</v>
       </c>
       <c r="D244" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8546,7 +8544,7 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C249" t="s">
         <v>19</v>
@@ -8566,7 +8564,7 @@
         <v>12</v>
       </c>
       <c r="D250" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8622,7 +8620,7 @@
         <v>38</v>
       </c>
       <c r="D254" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8644,7 +8642,7 @@
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C256" t="s">
         <v>19</v>
@@ -8672,7 +8670,7 @@
         <v>257</v>
       </c>
       <c r="B258" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C258" t="s">
         <v>19</v>
@@ -8692,7 +8690,7 @@
         <v>38</v>
       </c>
       <c r="D259" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8700,7 +8698,7 @@
         <v>259</v>
       </c>
       <c r="B260" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C260" t="s">
         <v>41</v>
@@ -8742,7 +8740,7 @@
         <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C263" t="s">
         <v>12</v>
@@ -8756,7 +8754,7 @@
         <v>263</v>
       </c>
       <c r="B264" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C264" t="s">
         <v>41</v>
@@ -8832,7 +8830,7 @@
         <v>5</v>
       </c>
       <c r="D269" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8840,7 +8838,7 @@
         <v>269</v>
       </c>
       <c r="B270" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C270" t="s">
         <v>5</v>
@@ -8854,7 +8852,7 @@
         <v>270</v>
       </c>
       <c r="B271" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C271" t="s">
         <v>41</v>
@@ -8910,7 +8908,7 @@
         <v>274</v>
       </c>
       <c r="B275" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C275" t="s">
         <v>19</v>
@@ -8952,13 +8950,13 @@
         <v>277</v>
       </c>
       <c r="B278" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C278" t="s">
         <v>5</v>
       </c>
       <c r="D278" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8966,7 +8964,7 @@
         <v>278</v>
       </c>
       <c r="B279" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C279" t="s">
         <v>19</v>
@@ -8994,7 +8992,7 @@
         <v>280</v>
       </c>
       <c r="B281" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C281" t="s">
         <v>41</v>
@@ -9014,7 +9012,7 @@
         <v>38</v>
       </c>
       <c r="D282" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9036,13 +9034,13 @@
         <v>283</v>
       </c>
       <c r="B284" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C284" t="s">
         <v>5</v>
       </c>
       <c r="D284" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9056,7 +9054,7 @@
         <v>12</v>
       </c>
       <c r="D285" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9064,7 +9062,7 @@
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C286" t="s">
         <v>5</v>
@@ -9084,7 +9082,7 @@
         <v>38</v>
       </c>
       <c r="D287" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9092,13 +9090,13 @@
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C288" t="s">
         <v>38</v>
       </c>
       <c r="D288" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9120,7 +9118,7 @@
         <v>289</v>
       </c>
       <c r="B290" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C290" t="s">
         <v>5</v>
@@ -9140,7 +9138,7 @@
         <v>12</v>
       </c>
       <c r="D291" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9148,7 +9146,7 @@
         <v>291</v>
       </c>
       <c r="B292" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C292" t="s">
         <v>38</v>
@@ -9218,7 +9216,7 @@
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C297" t="s">
         <v>41</v>
@@ -9232,13 +9230,13 @@
         <v>297</v>
       </c>
       <c r="B298" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C298" t="s">
         <v>38</v>
       </c>
       <c r="D298" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Fix filters and expand columns to fit content
</commit_message>
<xml_diff>
--- a/nhl-fantasy-rankings-2023.xlsx
+++ b/nhl-fantasy-rankings-2023.xlsx
@@ -13,10 +13,10 @@
     <sheet name="Average Rankings" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Average Rankings'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ESPN!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NHL.com'!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Yahoo!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Average Rankings'!$A$1:$B$501</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ESPN!$A$1:$D$301</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NHL.com'!$A$1:$D$301</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Yahoo!$A$1:$B$301</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1709,6 +1709,12 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -5225,7 +5231,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D301"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5237,6 +5243,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -9453,7 +9465,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D301"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9465,6 +9477,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -11875,7 +11891,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B301"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11887,6 +11903,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -15097,7 +15117,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B501"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>